<commit_message>
fix bug for upgrade building
</commit_message>
<xml_diff>
--- a/gameData/shared/Buildings.xlsx
+++ b/gameData/shared/Buildings.xlsx
@@ -36,9 +36,6 @@
     <t>warehouse</t>
   </si>
   <si>
-    <t>dragonEyire</t>
-  </si>
-  <si>
     <t>hospital</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
   <si>
     <t>false</t>
     <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>dragonEyrie</t>
   </si>
 </sst>
 </file>
@@ -834,7 +834,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="A1:D17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -846,16 +846,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -866,10 +866,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20" customHeight="1">
@@ -880,10 +880,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="20" customHeight="1">
@@ -894,10 +894,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="20" customHeight="1">
@@ -905,13 +905,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="20" customHeight="1">
@@ -919,13 +919,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="20" customHeight="1">
@@ -933,13 +933,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20" customHeight="1">
@@ -947,13 +947,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="20" customHeight="1">
@@ -961,13 +961,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="20" customHeight="1">
@@ -975,13 +975,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="20" customHeight="1">
@@ -989,13 +989,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="20" customHeight="1">
@@ -1003,13 +1003,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -1017,13 +1017,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="20" customHeight="1">
@@ -1031,13 +1031,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="20" customHeight="1">
@@ -1045,13 +1045,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="20" customHeight="1">
@@ -1059,13 +1059,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
@@ -1073,13 +1073,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fisnish dev of get march detail
</commit_message>
<xml_diff>
--- a/gameData/shared/Buildings.xlsx
+++ b/gameData/shared/Buildings.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-18320" yWindow="20" windowWidth="13640" windowHeight="15100" tabRatio="883"/>
+    <workbookView xWindow="6620" yWindow="1960" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="buildings" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>keep</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>materialDepot</t>
-  </si>
-  <si>
-    <t>armyCamp</t>
   </si>
   <si>
     <t>barracks</t>
@@ -94,9 +91,6 @@
     <t>材料库房</t>
   </si>
   <si>
-    <t>军用帐篷</t>
-  </si>
-  <si>
     <t>兵营</t>
   </si>
   <si>
@@ -152,10 +146,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>prison</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>hunterHall</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -172,35 +162,23 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>资源仓库</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>军用帐篷</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>贸易行会</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>监狱</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>猎手大厅</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>训练营地</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>马厩</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>车间</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>学院</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -354,7 +332,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -369,6 +347,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -431,7 +427,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="68">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -459,6 +455,15 @@
     <cellStyle name="超链接" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="66" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -479,6 +484,15 @@
     <cellStyle name="访问过的超链接" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -931,7 +945,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -943,16 +957,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -963,10 +977,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20" customHeight="1">
@@ -977,10 +991,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="20" customHeight="1">
@@ -991,10 +1005,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="20" customHeight="1">
@@ -1002,13 +1016,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="20" customHeight="1">
@@ -1016,13 +1030,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="20" customHeight="1">
@@ -1033,10 +1047,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20" customHeight="1">
@@ -1044,13 +1058,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="20" customHeight="1">
@@ -1058,13 +1072,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="20" customHeight="1">
@@ -1072,13 +1086,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="20" customHeight="1">
@@ -1086,13 +1100,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="20" customHeight="1">
@@ -1100,13 +1114,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -1114,13 +1128,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="20" customHeight="1">
@@ -1128,13 +1142,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="20" customHeight="1">
@@ -1145,10 +1159,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="20" customHeight="1">
@@ -1156,13 +1170,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
@@ -1170,13 +1184,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="20" customHeight="1">
@@ -1184,27 +1198,27 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="20" customHeight="1">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>2</v>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
@@ -1212,13 +1226,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20" customHeight="1">
@@ -1226,84 +1240,29 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="20" customHeight="1">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:4" ht="20" customHeight="1">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:4" ht="20" customHeight="1">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:4" ht="20" customHeight="1">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="C25" s="6"/>
     </row>
     <row r="26" spans="1:4" ht="20" customHeight="1">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="C26" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>

</xml_diff>

<commit_message>
finish dev of upgradeMilitaryTech
</commit_message>
<xml_diff>
--- a/gameData/shared/Buildings.xlsx
+++ b/gameData/shared/Buildings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6620" yWindow="1960" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
+    <workbookView xWindow="6960" yWindow="1660" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="buildings" sheetId="2" r:id="rId1"/>
@@ -138,10 +138,6 @@
     <t>dragonEyrie</t>
   </si>
   <si>
-    <t>STR_type</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>tradeGuild</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -182,7 +178,11 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>学院</t>
+    <t>训练场</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_name</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -332,7 +332,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="68">
+  <cellStyleXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -347,6 +347,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -427,7 +435,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="68">
+  <cellStyles count="76">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -464,6 +472,10 @@
     <cellStyle name="超链接" xfId="62" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="74" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -493,6 +505,10 @@
     <cellStyle name="访问过的超链接" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -944,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -960,7 +976,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>30</v>
@@ -1064,7 +1080,7 @@
         <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="20" customHeight="1">
@@ -1184,13 +1200,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="20" customHeight="1">
@@ -1198,13 +1214,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="20" customHeight="1">
@@ -1212,13 +1228,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
@@ -1226,13 +1242,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20" customHeight="1">
@@ -1240,13 +1256,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="20" customHeight="1">

</xml_diff>